<commit_message>
added close browser after all done
</commit_message>
<xml_diff>
--- a/Output/Output_IT_CVs.xlsx
+++ b/Output/Output_IT_CVs.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Ray\Ray PC Home\Raymond\Raymond Loh Wee Ping Resume\Race Academy\2021\Course Notes\RPA Projects\RPAJ01_JobMatchingForPlacements\Output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work\Desktop\Delta_RPAJ01_JobMatchingForPlacements - Copy\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DA5198-48CE-48DF-B0D9-A57B16EB8492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{34DDD9C4-B25B-4E4D-8771-E8077D4555D8}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>matchCVKeywords_col</t>
   </si>
@@ -36,85 +35,13 @@
     <t>matchCVCount_col</t>
   </si>
   <si>
-    <t>Change Management,SQL,JavaScript,Java,Database,Web Services,SQL Server,Linux,PHP,Python,HTML,Application Development,XML,Scripting,JQuery</t>
-  </si>
-  <si>
-    <t>C:\CVs\AllCVs\jeck P.docx</t>
-  </si>
-  <si>
-    <t>C:\CVs\AllCVs\Jennifer  M. Conte.docx</t>
-  </si>
-  <si>
-    <t>Engineering,SQL,JavaScript,Java,Database,Web Services,SQL Server,Linux,Software Development,HTML,XML,Scripting,JQuery</t>
-  </si>
-  <si>
-    <t>C:\CVs\AllCVs\jagadeesh k.docx</t>
-  </si>
-  <si>
-    <t>SQL,JavaScript,Java,Database,Web Services,SQL Server,Linux,Software Development,HTML,Application Development,XML,JQuery,Information Technology</t>
-  </si>
-  <si>
-    <t>C:\CVs\AllCVs\Jayadattaperi N.docx</t>
-  </si>
-  <si>
-    <t>Computer Science,SQL,Java,Database,Web Services,Software Development,Python,HTML,Application Development,XML,Scripting</t>
-  </si>
-  <si>
-    <t>C:\CVs\AllCVs\Jaya prakash.docx</t>
-  </si>
-  <si>
-    <t>Program Management,Change Management,Physics,SQL,HTML,Hardware,Information Technology</t>
-  </si>
-  <si>
-    <t>C:\CVs\AllCVs\Jagan S Iyer PM.docx</t>
-  </si>
-  <si>
-    <t>Engineering,Electronics,Database,Hardware,Information Technology</t>
-  </si>
-  <si>
-    <t>C:\CVs\AllCVs\1.pdf</t>
-  </si>
-  <si>
-    <t>Change Management,Engineering,SQL,Database,SQL Server</t>
-  </si>
-  <si>
-    <t>C:\CVs\AllCVs\Jimi_Desai_PM.docx</t>
-  </si>
-  <si>
-    <t>Engineering</t>
-  </si>
-  <si>
-    <t>C:\CVs\AllCVs\10.pdf</t>
-  </si>
-  <si>
-    <t>C:\CVs\AllCVs\2.pdf</t>
-  </si>
-  <si>
-    <t>Electronics</t>
-  </si>
-  <si>
-    <t>C:\CVs\AllCVs\4.pdf</t>
-  </si>
-  <si>
-    <t>C:\CVs\AllCVs\6.pdf</t>
-  </si>
-  <si>
-    <t>C:\CVs\AllCVs\7.pdf</t>
-  </si>
-  <si>
-    <t>HTML</t>
-  </si>
-  <si>
-    <t>C:\CVs\AllCVs\8.pdf</t>
-  </si>
-  <si>
     <t>matchCVPercentage_col</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -459,23 +386,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8022F09-6D2E-4D77-BA29-27D2CF7E9DC6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="127" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,202 +413,6 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>15</v>
-      </c>
-      <c r="D2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>15</v>
-      </c>
-      <c r="D3">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>7</v>
-      </c>
-      <c r="D7">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.75">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
         <v>3</v>
       </c>
     </row>

</xml_diff>